<commit_message>
apply python idiomatic refactor to classes
poner el return type con typing, usar logging para loguear en vez de print, poner el docstring para cada método con google style, etc
</commit_message>
<xml_diff>
--- a/resources/results/resultados_simulacion.xlsx
+++ b/resources/results/resultados_simulacion.xlsx
@@ -7,9 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q_ROUTING" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DIJKSTRA" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BELLMAN_FORD" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BELLMAN_FORD" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -492,217 +490,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D2" t="n">
-        <v>22</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>{}</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="9" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="17" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="17" customWidth="1" min="7" max="7"/>
-    <col width="16" customWidth="1" min="8" max="8"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>episode</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>start_time</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>end_time</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>episode_duration</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>episode_success</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>total_hops</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>dynamic_changes</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>packet_log_raw</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>29</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1510</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1481</v>
+        <v>17</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>296</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>{}</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="9" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="17" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="17" customWidth="1" min="7" max="7"/>
-    <col width="16" customWidth="1" min="8" max="8"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>episode</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>start_time</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>end_time</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>episode_duration</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>episode_success</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>total_hops</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>dynamic_changes</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>packet_log_raw</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1514</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2734</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1220</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>296</v>
+        <v>116</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>

</xml_diff>